<commit_message>
Correção da verificação de repetição, correção da base de repetição
Correção da verificação de repetição: Só considera repetição se for a mesma requisição e o mesmo motivo (Positivo, Negativo, Suspeito ou Nao Realizado)

Correção da base: Não fica colocando as colunas numéricas inúteis no início, que causava spam de coluna
</commit_message>
<xml_diff>
--- a/Gal Monitoramento 05.11.xlsx
+++ b/Gal Monitoramento 05.11.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Positivos" sheetId="1" r:id="rId1"/>
     <sheet name="Negativos" sheetId="2" r:id="rId2"/>
     <sheet name="Suspeitos" sheetId="3" r:id="rId3"/>
+    <sheet name="Não Realizados" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="213">
   <si>
     <t>RequisiCAo</t>
   </si>
@@ -177,6 +178,9 @@
     <t>DetectAvel</t>
   </si>
   <si>
+    <t>201410005877</t>
+  </si>
+  <si>
     <t>201410005888</t>
   </si>
   <si>
@@ -207,9 +211,27 @@
     <t>201410005980</t>
   </si>
   <si>
+    <t>201410005982</t>
+  </si>
+  <si>
+    <t>201410005993</t>
+  </si>
+  <si>
     <t>201410005994</t>
   </si>
   <si>
+    <t>201410005995</t>
+  </si>
+  <si>
+    <t>201410005996</t>
+  </si>
+  <si>
+    <t>201410006000</t>
+  </si>
+  <si>
+    <t>201410006004</t>
+  </si>
+  <si>
     <t>201410006007</t>
   </si>
   <si>
@@ -219,6 +241,9 @@
     <t>201410006104</t>
   </si>
   <si>
+    <t>LUCIANA APARECIDA DOS SANTOS</t>
+  </si>
+  <si>
     <t>VERA LUCIA DO AMARAL</t>
   </si>
   <si>
@@ -249,9 +274,27 @@
     <t>VIVIANE MARCAL DE OLIVEIRA</t>
   </si>
   <si>
+    <t>JOAO FLAVIO TAVEIRA</t>
+  </si>
+  <si>
+    <t>RODRIGO PEREIRA MIRANDA</t>
+  </si>
+  <si>
     <t>MATHEUS PIO DE ANDRADE DA SILVA</t>
   </si>
   <si>
+    <t>RAMON WILSON DE FREITAS</t>
+  </si>
+  <si>
+    <t>LUCIANA DE OLIVEIRA SANTOS</t>
+  </si>
+  <si>
+    <t>WELLINGTON MUNIZ COSTA</t>
+  </si>
+  <si>
+    <t>CARINA DE TOLEDO</t>
+  </si>
+  <si>
     <t>DANILO DONIZETE CATTO</t>
   </si>
   <si>
@@ -291,9 +334,27 @@
     <t>704806545946048</t>
   </si>
   <si>
+    <t>701801279369170</t>
+  </si>
+  <si>
+    <t>700203921278727</t>
+  </si>
+  <si>
     <t>707407007811971</t>
   </si>
   <si>
+    <t>165857166130001</t>
+  </si>
+  <si>
+    <t>122977962280009</t>
+  </si>
+  <si>
+    <t>702409042300121</t>
+  </si>
+  <si>
+    <t>200772437350000</t>
+  </si>
+  <si>
     <t>206859213060003</t>
   </si>
   <si>
@@ -333,9 +394,27 @@
     <t>21912069806</t>
   </si>
   <si>
+    <t>00571744826</t>
+  </si>
+  <si>
+    <t>41130364895</t>
+  </si>
+  <si>
     <t>42782308858</t>
   </si>
   <si>
+    <t>05019624179</t>
+  </si>
+  <si>
+    <t>17214269813</t>
+  </si>
+  <si>
+    <t>23714792848</t>
+  </si>
+  <si>
+    <t>35163741870</t>
+  </si>
+  <si>
     <t>34835376862</t>
   </si>
   <si>
@@ -360,63 +439,216 @@
     <t>UNIDADE BASICA DE SAUDE DR BARTOLOMEU MARAGLIANO VENERE</t>
   </si>
   <si>
+    <t>UNIDADE BASICA DE SAUDE DR LOTFALLAH MIZIARA</t>
+  </si>
+  <si>
     <t>UNIDADE BASICA ARCHIMEDES MACHADO DE BARRETOS</t>
   </si>
   <si>
     <t>NAo DetectAvel</t>
   </si>
   <si>
+    <t>201410005925</t>
+  </si>
+  <si>
+    <t>201410005929</t>
+  </si>
+  <si>
     <t>201410005939</t>
   </si>
   <si>
+    <t>201410005948</t>
+  </si>
+  <si>
+    <t>201410006044</t>
+  </si>
+  <si>
+    <t>201410006066</t>
+  </si>
+  <si>
     <t>201410006075</t>
   </si>
   <si>
+    <t>201410006082</t>
+  </si>
+  <si>
     <t>201410006115</t>
   </si>
   <si>
+    <t>201410006127</t>
+  </si>
+  <si>
+    <t>201410006153</t>
+  </si>
+  <si>
+    <t>201410006170</t>
+  </si>
+  <si>
+    <t>201410006171</t>
+  </si>
+  <si>
     <t>201410006188</t>
   </si>
   <si>
+    <t>201410006192</t>
+  </si>
+  <si>
+    <t>201410006195</t>
+  </si>
+  <si>
+    <t>ASSAD RAMADAN</t>
+  </si>
+  <si>
+    <t>GETULIO BERNARDINO DE PAULA NETO</t>
+  </si>
+  <si>
     <t>FRANCISCA ALVES DOS SANTOS</t>
   </si>
   <si>
+    <t>SERGIO ROBERTO BOVO</t>
+  </si>
+  <si>
+    <t>MARIA APARECIDA BALBINO</t>
+  </si>
+  <si>
+    <t>ANDREA CRISTINA ORTIZ MORELI</t>
+  </si>
+  <si>
     <t>DANIELI APARECIDA CARDOZO DA COSTA LEOVERGILIO</t>
   </si>
   <si>
+    <t>FLAVIO JERONIMO DA COSTA</t>
+  </si>
+  <si>
     <t>APARECIDA DA SILVA DE ARAUJO</t>
   </si>
   <si>
+    <t>ADRIEL HENRIQUE ALVES HONORATO</t>
+  </si>
+  <si>
+    <t>LUCIANO ALVES MARQUES</t>
+  </si>
+  <si>
+    <t>VIVIANE APARECIDA DA SILVA</t>
+  </si>
+  <si>
+    <t>ALEXANDRE APARECIDO VENDRAMIM</t>
+  </si>
+  <si>
     <t>ANA MARIA DE FREITAS</t>
   </si>
   <si>
+    <t>ISABELA MAIRA FERREIRA DA SILVA</t>
+  </si>
+  <si>
+    <t>LEONARDO MESSIAS FAUSTINO RIBEIRO</t>
+  </si>
+  <si>
+    <t>121435495570001</t>
+  </si>
+  <si>
+    <t>206563862010004</t>
+  </si>
+  <si>
     <t>124573837160008</t>
   </si>
   <si>
+    <t>708207618214849</t>
+  </si>
+  <si>
+    <t>164194365840004</t>
+  </si>
+  <si>
+    <t>124224880820018</t>
+  </si>
+  <si>
     <t>200439762920006</t>
   </si>
   <si>
+    <t>206356280010006</t>
+  </si>
+  <si>
     <t>702305146055015</t>
   </si>
   <si>
+    <t>203673544910006</t>
+  </si>
+  <si>
+    <t>708900774313716</t>
+  </si>
+  <si>
+    <t>704205716955989</t>
+  </si>
+  <si>
+    <t>706405676179589</t>
+  </si>
+  <si>
     <t>706806715507224</t>
   </si>
   <si>
+    <t>206424323110004</t>
+  </si>
+  <si>
+    <t>700009020885809</t>
+  </si>
+  <si>
+    <t>02653929856</t>
+  </si>
+  <si>
+    <t>36081991873</t>
+  </si>
+  <si>
     <t>14557804802</t>
   </si>
   <si>
+    <t>77406257872</t>
+  </si>
+  <si>
+    <t>23256423809</t>
+  </si>
+  <si>
+    <t>28890659874</t>
+  </si>
+  <si>
     <t>38046003875</t>
   </si>
   <si>
+    <t>31265247889</t>
+  </si>
+  <si>
     <t>15613193843</t>
   </si>
   <si>
+    <t>37539880813</t>
+  </si>
+  <si>
+    <t>26159518828</t>
+  </si>
+  <si>
+    <t>34937916823</t>
+  </si>
+  <si>
+    <t>29795003801</t>
+  </si>
+  <si>
     <t>06265451880</t>
   </si>
   <si>
+    <t>46228423860</t>
+  </si>
+  <si>
+    <t>43663596850</t>
+  </si>
+  <si>
     <t>UNIDADE BASICA DE SAUDE DR APOLONIO MORAES E SOUZA</t>
   </si>
   <si>
+    <t>FUNDACAO PIO XII BARRETOS</t>
+  </si>
+  <si>
+    <t>UNIDADE BASICA DE SAUDE DR PAULO PRATA</t>
+  </si>
+  <si>
     <t>UNIDADE BASICA DE SAUDE FRANCOLINO GALVAO DE SOUZA</t>
   </si>
   <si>
@@ -424,19 +656,16 @@
   </si>
   <si>
     <t>Aguardando Triagem</t>
-  </si>
-  <si>
-    <t>Já possui agravo no Assessor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -452,27 +681,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -502,33 +717,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -566,7 +773,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -600,7 +807,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -635,10 +841,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -811,23 +1016,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -904,51 +1100,92 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26">
+      <c r="A2" s="1">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2">
+        <v>350556949</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S2" s="2">
+        <v>44130.70174768518</v>
+      </c>
+      <c r="T2" s="2">
+        <v>44131.60586805556</v>
+      </c>
+      <c r="U2" s="2">
+        <v>44133.73163194444</v>
+      </c>
+      <c r="V2">
+        <v>2</v>
+      </c>
+      <c r="W2" t="s">
+        <v>50</v>
+      </c>
+      <c r="X2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3" s="1">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H3" t="s">
         <v>41</v>
@@ -957,7 +1194,7 @@
         <v>42</v>
       </c>
       <c r="J3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K3" t="s">
         <v>41</v>
@@ -972,7 +1209,7 @@
         <v>48</v>
       </c>
       <c r="O3">
-        <v>350556949</v>
+        <v>350578698</v>
       </c>
       <c r="P3">
         <v>1</v>
@@ -981,16 +1218,16 @@
         <v>49</v>
       </c>
       <c r="S3" s="2">
-        <v>44130.701747685183</v>
+        <v>44132.77607638889</v>
       </c>
       <c r="T3" s="2">
-        <v>44131.605868055558</v>
+        <v>44133.53355324074</v>
       </c>
       <c r="U3" s="2">
-        <v>44133.731631944444</v>
+        <v>44140.56517361111</v>
       </c>
       <c r="V3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="W3" t="s">
         <v>50</v>
@@ -1005,21 +1242,21 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26">
       <c r="A4" s="1">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H4" t="s">
         <v>41</v>
@@ -1028,7 +1265,7 @@
         <v>42</v>
       </c>
       <c r="J4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K4" t="s">
         <v>41</v>
@@ -1043,7 +1280,7 @@
         <v>48</v>
       </c>
       <c r="O4">
-        <v>350578698</v>
+        <v>350588384</v>
       </c>
       <c r="P4">
         <v>1</v>
@@ -1052,16 +1289,16 @@
         <v>49</v>
       </c>
       <c r="S4" s="2">
-        <v>44132.776076388887</v>
+        <v>44133.69069444444</v>
       </c>
       <c r="T4" s="2">
-        <v>44133.533553240741</v>
+        <v>44138.52212962963</v>
       </c>
       <c r="U4" s="2">
-        <v>44140.56517361111</v>
+        <v>44139.75354166667</v>
       </c>
       <c r="V4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="W4" t="s">
         <v>50</v>
@@ -1076,21 +1313,21 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26">
       <c r="A5" s="1">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H5" t="s">
         <v>41</v>
@@ -1099,7 +1336,7 @@
         <v>42</v>
       </c>
       <c r="J5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K5" t="s">
         <v>41</v>
@@ -1114,7 +1351,7 @@
         <v>48</v>
       </c>
       <c r="O5">
-        <v>350588384</v>
+        <v>350598710</v>
       </c>
       <c r="P5">
         <v>1</v>
@@ -1123,13 +1360,13 @@
         <v>49</v>
       </c>
       <c r="S5" s="2">
-        <v>44133.690694444442</v>
+        <v>44137.35810185185</v>
       </c>
       <c r="T5" s="2">
-        <v>44138.522129629629</v>
+        <v>44138.52907407407</v>
       </c>
       <c r="U5" s="2">
-        <v>44139.753541666672</v>
+        <v>44139.75244212963</v>
       </c>
       <c r="V5">
         <v>1</v>
@@ -1147,102 +1384,20 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>132</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" t="s">
-        <v>44</v>
-      </c>
-      <c r="K6" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" t="s">
-        <v>46</v>
-      </c>
-      <c r="M6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N6" t="s">
-        <v>48</v>
-      </c>
-      <c r="O6">
-        <v>350598710</v>
-      </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-      <c r="R6" t="s">
-        <v>49</v>
-      </c>
-      <c r="S6" s="2">
-        <v>44137.358101851853</v>
-      </c>
-      <c r="T6" s="2">
-        <v>44138.529074074067</v>
-      </c>
-      <c r="U6" s="2">
-        <v>44139.752442129633</v>
-      </c>
-      <c r="V6">
-        <v>1</v>
-      </c>
-      <c r="W6" t="s">
-        <v>50</v>
-      </c>
-      <c r="X6" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>52</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:Z2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1319,51 +1474,86 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2">
+        <v>350549586</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S2" s="2">
+        <v>44130.41479166667</v>
+      </c>
+      <c r="T2" s="2">
+        <v>44130.5497800926</v>
+      </c>
+      <c r="U2" s="2">
+        <v>44131.80813657407</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>50</v>
+      </c>
+      <c r="X2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3" s="1">
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="H3" t="s">
         <v>41</v>
@@ -1372,7 +1562,7 @@
         <v>42</v>
       </c>
       <c r="J3" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="K3" t="s">
         <v>41</v>
@@ -1396,13 +1586,13 @@
         <v>49</v>
       </c>
       <c r="S3" s="2">
-        <v>44130.651585648149</v>
+        <v>44130.65158564815</v>
       </c>
       <c r="T3" s="2">
-        <v>44131.600752314807</v>
+        <v>44131.60075231481</v>
       </c>
       <c r="U3" s="2">
-        <v>44133.732627314806</v>
+        <v>44133.73262731481</v>
       </c>
       <c r="V3">
         <v>2</v>
@@ -1414,27 +1604,27 @@
         <v>51</v>
       </c>
       <c r="Y3" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="Z3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" s="1">
         <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="H4" t="s">
         <v>41</v>
@@ -1443,7 +1633,7 @@
         <v>42</v>
       </c>
       <c r="J4" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="K4" t="s">
         <v>41</v>
@@ -1467,13 +1657,13 @@
         <v>49</v>
       </c>
       <c r="S4" s="2">
-        <v>44132.741215277783</v>
+        <v>44132.74121527778</v>
       </c>
       <c r="T4" s="2">
-        <v>44133.533020833333</v>
+        <v>44133.53302083333</v>
       </c>
       <c r="U4" s="2">
-        <v>44140.562800925924</v>
+        <v>44140.56280092592</v>
       </c>
       <c r="V4">
         <v>7</v>
@@ -1485,27 +1675,27 @@
         <v>51</v>
       </c>
       <c r="Y4" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="Z4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5" s="1">
         <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="H5" t="s">
         <v>41</v>
@@ -1538,13 +1728,13 @@
         <v>49</v>
       </c>
       <c r="S5" s="2">
-        <v>44132.743275462963</v>
+        <v>44132.74327546296</v>
       </c>
       <c r="T5" s="2">
-        <v>44133.533020833333</v>
+        <v>44133.53302083333</v>
       </c>
       <c r="U5" s="2">
-        <v>44140.566504629627</v>
+        <v>44140.56650462963</v>
       </c>
       <c r="V5">
         <v>7</v>
@@ -1556,27 +1746,27 @@
         <v>51</v>
       </c>
       <c r="Y5" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="Z5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
       <c r="A6" s="1">
         <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="E6" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="H6" t="s">
         <v>41</v>
@@ -1609,13 +1799,13 @@
         <v>49</v>
       </c>
       <c r="S6" s="2">
-        <v>44132.774212962962</v>
+        <v>44132.77421296296</v>
       </c>
       <c r="T6" s="2">
-        <v>44133.533553240741</v>
+        <v>44133.53355324074</v>
       </c>
       <c r="U6" s="2">
-        <v>44139.474085648151</v>
+        <v>44139.47408564815</v>
       </c>
       <c r="V6">
         <v>6</v>
@@ -1627,27 +1817,27 @@
         <v>51</v>
       </c>
       <c r="Y6" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="Z6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
       <c r="A7" s="1">
         <v>80</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="E7" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="H7" t="s">
         <v>41</v>
@@ -1656,7 +1846,7 @@
         <v>42</v>
       </c>
       <c r="J7" t="s">
-        <v>111</v>
+        <v>137</v>
       </c>
       <c r="K7" t="s">
         <v>41</v>
@@ -1680,13 +1870,13 @@
         <v>49</v>
       </c>
       <c r="S7" s="2">
-        <v>44132.780219907407</v>
+        <v>44132.78021990741</v>
       </c>
       <c r="T7" s="2">
-        <v>44133.533553240741</v>
+        <v>44133.53355324074</v>
       </c>
       <c r="U7" s="2">
-        <v>44140.566296296303</v>
+        <v>44140.5662962963</v>
       </c>
       <c r="V7">
         <v>7</v>
@@ -1698,27 +1888,27 @@
         <v>51</v>
       </c>
       <c r="Y7" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="Z7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
       <c r="A8" s="1">
         <v>81</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="H8" t="s">
         <v>41</v>
@@ -1751,13 +1941,13 @@
         <v>49</v>
       </c>
       <c r="S8" s="2">
-        <v>44132.781990740739</v>
+        <v>44132.78199074074</v>
       </c>
       <c r="T8" s="2">
-        <v>44133.533553240741</v>
+        <v>44133.53355324074</v>
       </c>
       <c r="U8" s="2">
-        <v>44139.474178240736</v>
+        <v>44139.47417824074</v>
       </c>
       <c r="V8">
         <v>6</v>
@@ -1769,27 +1959,27 @@
         <v>51</v>
       </c>
       <c r="Y8" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="Z8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
       <c r="A9" s="1">
         <v>85</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D9" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="E9" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="H9" t="s">
         <v>41</v>
@@ -1798,7 +1988,7 @@
         <v>42</v>
       </c>
       <c r="J9" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="K9" t="s">
         <v>41</v>
@@ -1825,10 +2015,10 @@
         <v>44132.79005787037</v>
       </c>
       <c r="T9" s="2">
-        <v>44133.533773148149</v>
+        <v>44133.53377314815</v>
       </c>
       <c r="U9" s="2">
-        <v>44139.474606481483</v>
+        <v>44139.47460648148</v>
       </c>
       <c r="V9">
         <v>6</v>
@@ -1840,27 +2030,27 @@
         <v>51</v>
       </c>
       <c r="Y9" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="Z9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
       <c r="A10" s="1">
         <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D10" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="E10" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="H10" t="s">
         <v>41</v>
@@ -1869,7 +2059,7 @@
         <v>42</v>
       </c>
       <c r="J10" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="K10" t="s">
         <v>41</v>
@@ -1896,10 +2086,10 @@
         <v>44133.68677083333</v>
       </c>
       <c r="T10" s="2">
-        <v>44138.522129629629</v>
+        <v>44138.52212962963</v>
       </c>
       <c r="U10" s="2">
-        <v>44139.753541666672</v>
+        <v>44139.75354166667</v>
       </c>
       <c r="V10">
         <v>1</v>
@@ -1911,27 +2101,27 @@
         <v>51</v>
       </c>
       <c r="Y10" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="Z10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
       <c r="A11" s="1">
         <v>95</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D11" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="E11" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="H11" t="s">
         <v>41</v>
@@ -1964,13 +2154,13 @@
         <v>49</v>
       </c>
       <c r="S11" s="2">
-        <v>44133.694293981483</v>
+        <v>44133.69429398148</v>
       </c>
       <c r="T11" s="2">
-        <v>44138.522129629629</v>
+        <v>44138.52212962963</v>
       </c>
       <c r="U11" s="2">
-        <v>44139.753530092603</v>
+        <v>44139.7535300926</v>
       </c>
       <c r="V11">
         <v>1</v>
@@ -1982,27 +2172,27 @@
         <v>51</v>
       </c>
       <c r="Y11" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="Z11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
       <c r="A12" s="1">
         <v>98</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="E12" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="H12" t="s">
         <v>41</v>
@@ -2035,13 +2225,13 @@
         <v>49</v>
       </c>
       <c r="S12" s="2">
-        <v>44133.700937499998</v>
+        <v>44133.7009375</v>
       </c>
       <c r="T12" s="2">
-        <v>44138.522141203714</v>
+        <v>44138.52214120371</v>
       </c>
       <c r="U12" s="2">
-        <v>44139.753518518519</v>
+        <v>44139.75351851852</v>
       </c>
       <c r="V12">
         <v>1</v>
@@ -2053,27 +2243,27 @@
         <v>51</v>
       </c>
       <c r="Y12" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="Z12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
       <c r="A13" s="1">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="E13" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="H13" t="s">
         <v>41</v>
@@ -2082,7 +2272,7 @@
         <v>42</v>
       </c>
       <c r="J13" t="s">
-        <v>113</v>
+        <v>43</v>
       </c>
       <c r="K13" t="s">
         <v>41</v>
@@ -2097,7 +2287,7 @@
         <v>48</v>
       </c>
       <c r="O13">
-        <v>350588974</v>
+        <v>350588508</v>
       </c>
       <c r="P13">
         <v>1</v>
@@ -2106,13 +2296,13 @@
         <v>49</v>
       </c>
       <c r="S13" s="2">
-        <v>44133.744733796288</v>
+        <v>44133.70407407408</v>
       </c>
       <c r="T13" s="2">
-        <v>44138.527557870373</v>
+        <v>44138.52230324074</v>
       </c>
       <c r="U13" s="2">
-        <v>44139.753252314818</v>
+        <v>44139.75351851852</v>
       </c>
       <c r="V13">
         <v>1</v>
@@ -2124,27 +2314,27 @@
         <v>51</v>
       </c>
       <c r="Y13" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="Z13" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
       <c r="A14" s="1">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D14" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="E14" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="H14" t="s">
         <v>41</v>
@@ -2153,7 +2343,7 @@
         <v>42</v>
       </c>
       <c r="J14" t="s">
-        <v>44</v>
+        <v>139</v>
       </c>
       <c r="K14" t="s">
         <v>41</v>
@@ -2168,7 +2358,7 @@
         <v>48</v>
       </c>
       <c r="O14">
-        <v>350598553</v>
+        <v>350588952</v>
       </c>
       <c r="P14">
         <v>1</v>
@@ -2177,13 +2367,13 @@
         <v>49</v>
       </c>
       <c r="S14" s="2">
-        <v>44137.339444444442</v>
+        <v>44133.7427662037</v>
       </c>
       <c r="T14" s="2">
-        <v>44138.528101851851</v>
+        <v>44138.52755787037</v>
       </c>
       <c r="U14" s="2">
-        <v>44139.753229166658</v>
+        <v>44139.75325231482</v>
       </c>
       <c r="V14">
         <v>1</v>
@@ -2195,27 +2385,27 @@
         <v>51</v>
       </c>
       <c r="Y14" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="Z14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
       <c r="A15" s="1">
+        <v>112</v>
+      </c>
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" t="s">
         <v>127</v>
-      </c>
-      <c r="B15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" t="s">
-        <v>93</v>
-      </c>
-      <c r="E15" t="s">
-        <v>107</v>
       </c>
       <c r="H15" t="s">
         <v>41</v>
@@ -2224,7 +2414,7 @@
         <v>42</v>
       </c>
       <c r="J15" t="s">
-        <v>44</v>
+        <v>139</v>
       </c>
       <c r="K15" t="s">
         <v>41</v>
@@ -2239,7 +2429,7 @@
         <v>48</v>
       </c>
       <c r="O15">
-        <v>350598585</v>
+        <v>350588974</v>
       </c>
       <c r="P15">
         <v>1</v>
@@ -2248,13 +2438,13 @@
         <v>49</v>
       </c>
       <c r="S15" s="2">
-        <v>44137.343935185178</v>
+        <v>44133.74473379629</v>
       </c>
       <c r="T15" s="2">
-        <v>44138.529062499998</v>
+        <v>44138.52755787037</v>
       </c>
       <c r="U15" s="2">
-        <v>44139.753229166658</v>
+        <v>44139.75325231482</v>
       </c>
       <c r="V15">
         <v>1</v>
@@ -2266,27 +2456,27 @@
         <v>51</v>
       </c>
       <c r="Y15" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="Z15" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
       <c r="A16" s="1">
-        <v>222</v>
+        <v>113</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D16" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="H16" t="s">
         <v>41</v>
@@ -2295,7 +2485,7 @@
         <v>42</v>
       </c>
       <c r="J16" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="K16" t="s">
         <v>41</v>
@@ -2310,7 +2500,7 @@
         <v>48</v>
       </c>
       <c r="O16">
-        <v>350602288</v>
+        <v>350588994</v>
       </c>
       <c r="P16">
         <v>1</v>
@@ -2319,13 +2509,13 @@
         <v>49</v>
       </c>
       <c r="S16" s="2">
-        <v>44138.365810185183</v>
+        <v>44133.74626157407</v>
       </c>
       <c r="T16" s="2">
-        <v>44138.529780092591</v>
+        <v>44138.52755787037</v>
       </c>
       <c r="U16" s="2">
-        <v>44139.752430555563</v>
+        <v>44139.75325231482</v>
       </c>
       <c r="V16">
         <v>1</v>
@@ -2337,36 +2527,452 @@
         <v>51</v>
       </c>
       <c r="Y16" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="Z16" t="s">
-        <v>115</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26">
+      <c r="A17" s="1">
+        <v>114</v>
+      </c>
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" t="s">
+        <v>129</v>
+      </c>
+      <c r="H17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" t="s">
+        <v>140</v>
+      </c>
+      <c r="K17" t="s">
+        <v>41</v>
+      </c>
+      <c r="L17" t="s">
+        <v>46</v>
+      </c>
+      <c r="M17" t="s">
+        <v>47</v>
+      </c>
+      <c r="N17" t="s">
+        <v>48</v>
+      </c>
+      <c r="O17">
+        <v>350589008</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="R17" t="s">
+        <v>49</v>
+      </c>
+      <c r="S17" s="2">
+        <v>44133.74774305556</v>
+      </c>
+      <c r="T17" s="2">
+        <v>44138.52755787037</v>
+      </c>
+      <c r="U17" s="2">
+        <v>44139.75325231482</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17" t="s">
+        <v>50</v>
+      </c>
+      <c r="X17" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
+      <c r="A18" s="1">
+        <v>118</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" t="s">
+        <v>110</v>
+      </c>
+      <c r="E18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" t="s">
+        <v>140</v>
+      </c>
+      <c r="K18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L18" t="s">
+        <v>46</v>
+      </c>
+      <c r="M18" t="s">
+        <v>47</v>
+      </c>
+      <c r="N18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O18">
+        <v>350589080</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="R18" t="s">
+        <v>49</v>
+      </c>
+      <c r="S18" s="2">
+        <v>44133.75475694444</v>
+      </c>
+      <c r="T18" s="2">
+        <v>44138.52809027778</v>
+      </c>
+      <c r="U18" s="2">
+        <v>44139.75324074074</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18" t="s">
+        <v>50</v>
+      </c>
+      <c r="X18" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26">
+      <c r="A19" s="1">
+        <v>122</v>
+      </c>
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" t="s">
+        <v>131</v>
+      </c>
+      <c r="H19" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" t="s">
+        <v>141</v>
+      </c>
+      <c r="K19" t="s">
+        <v>41</v>
+      </c>
+      <c r="L19" t="s">
+        <v>46</v>
+      </c>
+      <c r="M19" t="s">
+        <v>47</v>
+      </c>
+      <c r="N19" t="s">
+        <v>48</v>
+      </c>
+      <c r="O19">
+        <v>350589134</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="R19" t="s">
+        <v>49</v>
+      </c>
+      <c r="S19" s="2">
+        <v>44133.76166666667</v>
+      </c>
+      <c r="T19" s="2">
+        <v>44138.52809027778</v>
+      </c>
+      <c r="U19" s="2">
+        <v>44139.75324074074</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="W19" t="s">
+        <v>50</v>
+      </c>
+      <c r="X19" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26">
+      <c r="A20" s="1">
+        <v>125</v>
+      </c>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" t="s">
+        <v>132</v>
+      </c>
+      <c r="H20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K20" t="s">
+        <v>41</v>
+      </c>
+      <c r="L20" t="s">
+        <v>46</v>
+      </c>
+      <c r="M20" t="s">
+        <v>47</v>
+      </c>
+      <c r="N20" t="s">
+        <v>48</v>
+      </c>
+      <c r="O20">
+        <v>350598553</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="R20" t="s">
+        <v>49</v>
+      </c>
+      <c r="S20" s="2">
+        <v>44137.33944444444</v>
+      </c>
+      <c r="T20" s="2">
+        <v>44138.52810185185</v>
+      </c>
+      <c r="U20" s="2">
+        <v>44139.75322916666</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="W20" t="s">
+        <v>50</v>
+      </c>
+      <c r="X20" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26">
+      <c r="A21" s="1">
+        <v>127</v>
+      </c>
+      <c r="B21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" t="s">
+        <v>133</v>
+      </c>
+      <c r="H21" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" t="s">
+        <v>42</v>
+      </c>
+      <c r="J21" t="s">
+        <v>44</v>
+      </c>
+      <c r="K21" t="s">
+        <v>41</v>
+      </c>
+      <c r="L21" t="s">
+        <v>46</v>
+      </c>
+      <c r="M21" t="s">
+        <v>47</v>
+      </c>
+      <c r="N21" t="s">
+        <v>48</v>
+      </c>
+      <c r="O21">
+        <v>350598585</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="R21" t="s">
+        <v>49</v>
+      </c>
+      <c r="S21" s="2">
+        <v>44137.34393518518</v>
+      </c>
+      <c r="T21" s="2">
+        <v>44138.5290625</v>
+      </c>
+      <c r="U21" s="2">
+        <v>44139.75322916666</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21" t="s">
+        <v>50</v>
+      </c>
+      <c r="X21" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26">
+      <c r="A22" s="1">
+        <v>222</v>
+      </c>
+      <c r="B22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" t="s">
+        <v>134</v>
+      </c>
+      <c r="H22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I22" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" t="s">
+        <v>141</v>
+      </c>
+      <c r="K22" t="s">
+        <v>41</v>
+      </c>
+      <c r="L22" t="s">
+        <v>46</v>
+      </c>
+      <c r="M22" t="s">
+        <v>47</v>
+      </c>
+      <c r="N22" t="s">
+        <v>48</v>
+      </c>
+      <c r="O22">
+        <v>350602288</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="R22" t="s">
+        <v>49</v>
+      </c>
+      <c r="S22" s="2">
+        <v>44138.36581018518</v>
+      </c>
+      <c r="T22" s="2">
+        <v>44138.52978009259</v>
+      </c>
+      <c r="U22" s="2">
+        <v>44139.75243055556</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22" t="s">
+        <v>50</v>
+      </c>
+      <c r="X22" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:Z2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2443,21 +3049,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26">
       <c r="A2" s="1">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s">
-        <v>120</v>
+        <v>159</v>
       </c>
       <c r="D2" t="s">
-        <v>124</v>
+        <v>175</v>
       </c>
       <c r="E2" t="s">
-        <v>128</v>
+        <v>191</v>
       </c>
       <c r="H2" t="s">
         <v>41</v>
@@ -2466,7 +3072,7 @@
         <v>42</v>
       </c>
       <c r="J2" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="K2" t="s">
         <v>41</v>
@@ -2481,7 +3087,7 @@
         <v>48</v>
       </c>
       <c r="O2">
-        <v>350568093</v>
+        <v>350567245</v>
       </c>
       <c r="P2">
         <v>1</v>
@@ -2490,30 +3096,30 @@
         <v>49</v>
       </c>
       <c r="S2" s="2">
-        <v>44131.707789351851</v>
+        <v>44131.64851851852</v>
       </c>
       <c r="T2" s="2">
-        <v>44132.590115740742</v>
+        <v>44132.58804398148</v>
       </c>
       <c r="X2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3" s="1">
-        <v>193</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>160</v>
       </c>
       <c r="D3" t="s">
-        <v>125</v>
+        <v>176</v>
       </c>
       <c r="E3" t="s">
-        <v>129</v>
+        <v>192</v>
       </c>
       <c r="H3" t="s">
         <v>41</v>
@@ -2522,7 +3128,7 @@
         <v>42</v>
       </c>
       <c r="J3" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="K3" t="s">
         <v>41</v>
@@ -2537,7 +3143,7 @@
         <v>48</v>
       </c>
       <c r="O3">
-        <v>350600328</v>
+        <v>350567407</v>
       </c>
       <c r="P3">
         <v>1</v>
@@ -2546,27 +3152,30 @@
         <v>49</v>
       </c>
       <c r="S3" s="2">
-        <v>44137.792615740742</v>
+        <v>44131.65592592592</v>
+      </c>
+      <c r="T3" s="2">
+        <v>44132.58928240741</v>
       </c>
       <c r="X3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" s="1">
-        <v>232</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="C4" t="s">
-        <v>122</v>
+        <v>161</v>
       </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>177</v>
       </c>
       <c r="E4" t="s">
-        <v>130</v>
+        <v>193</v>
       </c>
       <c r="H4" t="s">
         <v>41</v>
@@ -2575,7 +3184,7 @@
         <v>42</v>
       </c>
       <c r="J4" t="s">
-        <v>132</v>
+        <v>207</v>
       </c>
       <c r="K4" t="s">
         <v>41</v>
@@ -2590,7 +3199,7 @@
         <v>48</v>
       </c>
       <c r="O4">
-        <v>350609467</v>
+        <v>350568093</v>
       </c>
       <c r="P4">
         <v>1</v>
@@ -2599,30 +3208,30 @@
         <v>49</v>
       </c>
       <c r="S4" s="2">
-        <v>44138.673113425917</v>
+        <v>44131.70778935185</v>
       </c>
       <c r="T4" s="2">
-        <v>44139.613530092603</v>
+        <v>44132.59011574074</v>
       </c>
       <c r="X4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5" s="1">
-        <v>303</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="D5" t="s">
-        <v>127</v>
+        <v>178</v>
       </c>
       <c r="E5" t="s">
-        <v>131</v>
+        <v>194</v>
       </c>
       <c r="H5" t="s">
         <v>41</v>
@@ -2631,7 +3240,7 @@
         <v>42</v>
       </c>
       <c r="J5" t="s">
-        <v>133</v>
+        <v>208</v>
       </c>
       <c r="K5" t="s">
         <v>41</v>
@@ -2646,7 +3255,7 @@
         <v>48</v>
       </c>
       <c r="O5">
-        <v>350632737</v>
+        <v>350570759</v>
       </c>
       <c r="P5">
         <v>1</v>
@@ -2655,10 +3264,754 @@
         <v>49</v>
       </c>
       <c r="S5" s="2">
-        <v>44140.695648148147</v>
+        <v>44132.35644675926</v>
+      </c>
+      <c r="T5" s="2">
+        <v>44132.59155092593</v>
       </c>
       <c r="X5" t="s">
-        <v>135</v>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" s="1">
+        <v>162</v>
+      </c>
+      <c r="B6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6" t="s">
+        <v>195</v>
+      </c>
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" t="s">
+        <v>139</v>
+      </c>
+      <c r="K6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N6" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6">
+        <v>350600102</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="R6" t="s">
+        <v>49</v>
+      </c>
+      <c r="S6" s="2">
+        <v>44137.71671296296</v>
+      </c>
+      <c r="X6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" s="1">
+        <v>184</v>
+      </c>
+      <c r="B7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E7" t="s">
+        <v>196</v>
+      </c>
+      <c r="H7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" t="s">
+        <v>139</v>
+      </c>
+      <c r="K7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7">
+        <v>350600241</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="R7" t="s">
+        <v>49</v>
+      </c>
+      <c r="S7" s="2">
+        <v>44137.76998842593</v>
+      </c>
+      <c r="X7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" s="1">
+        <v>193</v>
+      </c>
+      <c r="B8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" t="s">
+        <v>181</v>
+      </c>
+      <c r="E8" t="s">
+        <v>197</v>
+      </c>
+      <c r="H8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" t="s">
+        <v>139</v>
+      </c>
+      <c r="K8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N8" t="s">
+        <v>48</v>
+      </c>
+      <c r="O8">
+        <v>350600328</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
+        <v>49</v>
+      </c>
+      <c r="S8" s="2">
+        <v>44137.79261574074</v>
+      </c>
+      <c r="X8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" s="1">
+        <v>200</v>
+      </c>
+      <c r="B9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D9" t="s">
+        <v>182</v>
+      </c>
+      <c r="E9" t="s">
+        <v>198</v>
+      </c>
+      <c r="H9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" t="s">
+        <v>139</v>
+      </c>
+      <c r="K9" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N9" t="s">
+        <v>48</v>
+      </c>
+      <c r="O9">
+        <v>350600353</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="R9" t="s">
+        <v>49</v>
+      </c>
+      <c r="S9" s="2">
+        <v>44137.81282407408</v>
+      </c>
+      <c r="X9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" s="1">
+        <v>232</v>
+      </c>
+      <c r="B10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" t="s">
+        <v>167</v>
+      </c>
+      <c r="D10" t="s">
+        <v>183</v>
+      </c>
+      <c r="E10" t="s">
+        <v>199</v>
+      </c>
+      <c r="H10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" t="s">
+        <v>207</v>
+      </c>
+      <c r="K10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" t="s">
+        <v>46</v>
+      </c>
+      <c r="M10" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" t="s">
+        <v>48</v>
+      </c>
+      <c r="O10">
+        <v>350609467</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="R10" t="s">
+        <v>49</v>
+      </c>
+      <c r="S10" s="2">
+        <v>44138.67311342592</v>
+      </c>
+      <c r="T10" s="2">
+        <v>44139.6135300926</v>
+      </c>
+      <c r="X10" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" s="1">
+        <v>244</v>
+      </c>
+      <c r="B11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" t="s">
+        <v>168</v>
+      </c>
+      <c r="D11" t="s">
+        <v>184</v>
+      </c>
+      <c r="E11" t="s">
+        <v>200</v>
+      </c>
+      <c r="H11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K11" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M11" t="s">
+        <v>47</v>
+      </c>
+      <c r="N11" t="s">
+        <v>48</v>
+      </c>
+      <c r="O11">
+        <v>350609908</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="R11" t="s">
+        <v>49</v>
+      </c>
+      <c r="S11" s="2">
+        <v>44138.69766203704</v>
+      </c>
+      <c r="T11" s="2">
+        <v>44139.61484953704</v>
+      </c>
+      <c r="X11" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12" s="1">
+        <v>270</v>
+      </c>
+      <c r="B12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" t="s">
+        <v>169</v>
+      </c>
+      <c r="D12" t="s">
+        <v>185</v>
+      </c>
+      <c r="E12" t="s">
+        <v>201</v>
+      </c>
+      <c r="H12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" t="s">
+        <v>41</v>
+      </c>
+      <c r="L12" t="s">
+        <v>46</v>
+      </c>
+      <c r="M12" t="s">
+        <v>47</v>
+      </c>
+      <c r="N12" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12">
+        <v>350621276</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="R12" t="s">
+        <v>49</v>
+      </c>
+      <c r="S12" s="2">
+        <v>44139.73466435185</v>
+      </c>
+      <c r="T12" s="2">
+        <v>44140.62109953703</v>
+      </c>
+      <c r="X12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13" s="1">
+        <v>287</v>
+      </c>
+      <c r="B13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" t="s">
+        <v>170</v>
+      </c>
+      <c r="D13" t="s">
+        <v>186</v>
+      </c>
+      <c r="E13" t="s">
+        <v>202</v>
+      </c>
+      <c r="H13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" t="s">
+        <v>209</v>
+      </c>
+      <c r="K13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L13" t="s">
+        <v>46</v>
+      </c>
+      <c r="M13" t="s">
+        <v>47</v>
+      </c>
+      <c r="N13" t="s">
+        <v>48</v>
+      </c>
+      <c r="O13">
+        <v>350621522</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="R13" t="s">
+        <v>49</v>
+      </c>
+      <c r="S13" s="2">
+        <v>44139.76458333333</v>
+      </c>
+      <c r="T13" s="2">
+        <v>44140.62332175926</v>
+      </c>
+      <c r="X13" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" s="1">
+        <v>288</v>
+      </c>
+      <c r="B14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" t="s">
+        <v>171</v>
+      </c>
+      <c r="D14" t="s">
+        <v>187</v>
+      </c>
+      <c r="E14" t="s">
+        <v>203</v>
+      </c>
+      <c r="H14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" t="s">
+        <v>209</v>
+      </c>
+      <c r="K14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L14" t="s">
+        <v>46</v>
+      </c>
+      <c r="M14" t="s">
+        <v>47</v>
+      </c>
+      <c r="N14" t="s">
+        <v>48</v>
+      </c>
+      <c r="O14">
+        <v>350621535</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="R14" t="s">
+        <v>49</v>
+      </c>
+      <c r="S14" s="2">
+        <v>44139.76609953704</v>
+      </c>
+      <c r="T14" s="2">
+        <v>44140.62332175926</v>
+      </c>
+      <c r="X14" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" s="1">
+        <v>303</v>
+      </c>
+      <c r="B15" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" t="s">
+        <v>172</v>
+      </c>
+      <c r="D15" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" t="s">
+        <v>204</v>
+      </c>
+      <c r="H15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" t="s">
+        <v>210</v>
+      </c>
+      <c r="K15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L15" t="s">
+        <v>46</v>
+      </c>
+      <c r="M15" t="s">
+        <v>47</v>
+      </c>
+      <c r="N15" t="s">
+        <v>48</v>
+      </c>
+      <c r="O15">
+        <v>350632737</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="R15" t="s">
+        <v>49</v>
+      </c>
+      <c r="S15" s="2">
+        <v>44140.69564814815</v>
+      </c>
+      <c r="X15" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" s="1">
+        <v>307</v>
+      </c>
+      <c r="B16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" t="s">
+        <v>173</v>
+      </c>
+      <c r="D16" t="s">
+        <v>189</v>
+      </c>
+      <c r="E16" t="s">
+        <v>205</v>
+      </c>
+      <c r="H16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" t="s">
+        <v>41</v>
+      </c>
+      <c r="L16" t="s">
+        <v>46</v>
+      </c>
+      <c r="M16" t="s">
+        <v>47</v>
+      </c>
+      <c r="N16" t="s">
+        <v>48</v>
+      </c>
+      <c r="O16">
+        <v>350632865</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="R16" t="s">
+        <v>49</v>
+      </c>
+      <c r="S16" s="2">
+        <v>44140.70519675926</v>
+      </c>
+      <c r="X16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24">
+      <c r="A17" s="1">
+        <v>310</v>
+      </c>
+      <c r="B17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D17" t="s">
+        <v>190</v>
+      </c>
+      <c r="E17" t="s">
+        <v>206</v>
+      </c>
+      <c r="H17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" t="s">
+        <v>140</v>
+      </c>
+      <c r="K17" t="s">
+        <v>41</v>
+      </c>
+      <c r="L17" t="s">
+        <v>46</v>
+      </c>
+      <c r="M17" t="s">
+        <v>47</v>
+      </c>
+      <c r="N17" t="s">
+        <v>48</v>
+      </c>
+      <c r="O17">
+        <v>350632950</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="R17" t="s">
+        <v>49</v>
+      </c>
+      <c r="S17" s="2">
+        <v>44140.71136574074</v>
+      </c>
+      <c r="X17" t="s">
+        <v>212</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:Z1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:26">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>